<commit_message>
caricamento Excel via resource
</commit_message>
<xml_diff>
--- a/cart.test/src/main/resources/Configuratore.xlsx
+++ b/cart.test/src/main/resources/Configuratore.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CLLEGA" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,67 +23,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <authors>
-    <author> </author>
-  </authors>
-  <commentList>
-    <comment ref="A2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">name: tipcf110.copt
-type: string
-primaryKey: true
-session: tipcf1110m000</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">name: tipcf110.copt
-type: string
-primaryKey: true
-session: tipcf1110m000</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">name: tipcf110.copt
-type: string
-primaryKey: true
-session: tipcf1110m000</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -148,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="175">
   <si>
     <t xml:space="preserve">1A</t>
   </si>
@@ -376,18 +315,6 @@
   </si>
   <si>
     <t xml:space="preserve">[mm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 - CLSTATF - Stato Fisico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Opzione</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descrizione</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vincolo</t>
   </si>
   <si>
     <t xml:space="preserve">H00</t>
@@ -561,6 +488,15 @@
   </si>
   <si>
     <t xml:space="preserve">4 - CLFINI - Finitura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opzione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descrizione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vincolo</t>
   </si>
   <si>
     <t xml:space="preserve">7U1</t>
@@ -886,7 +822,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -909,14 +845,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -954,11 +882,11 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.57"/>
@@ -1276,7 +1204,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="2" width="12.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="9.14"/>
@@ -1333,209 +1261,209 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="73"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="A2" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>82</v>
-      </c>
+      <c r="C3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="8"/>
+        <v>82</v>
+      </c>
+      <c r="C4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="C5" s="8"/>
+        <v>83</v>
+      </c>
+      <c r="C5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="C6" s="8"/>
+        <v>84</v>
+      </c>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="C7" s="8"/>
+        <v>85</v>
+      </c>
+      <c r="C7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="C8" s="8"/>
+        <v>86</v>
+      </c>
+      <c r="C8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="C9" s="8"/>
+        <v>87</v>
+      </c>
+      <c r="C9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="C10" s="8"/>
+        <v>88</v>
+      </c>
+      <c r="C10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="C11" s="8"/>
+        <v>89</v>
+      </c>
+      <c r="C11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="C12" s="8"/>
+        <v>90</v>
+      </c>
+      <c r="C12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="C13" s="8"/>
+        <v>91</v>
+      </c>
+      <c r="C13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="C14" s="8"/>
+        <v>92</v>
+      </c>
+      <c r="C14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="C15" s="8"/>
+        <v>93</v>
+      </c>
+      <c r="C15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" s="8"/>
+        <v>94</v>
+      </c>
+      <c r="C16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="C17" s="8"/>
+        <v>95</v>
+      </c>
+      <c r="C17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="C18" s="8"/>
+        <v>96</v>
+      </c>
+      <c r="C18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="C19" s="8"/>
+        <v>97</v>
+      </c>
+      <c r="C19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="C20" s="8"/>
+        <v>99</v>
+      </c>
+      <c r="C20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="C21" s="8"/>
+      <c r="C21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
@@ -1544,7 +1472,7 @@
       <c r="B22" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="C22" s="8"/>
+      <c r="C22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
@@ -1553,159 +1481,142 @@
       <c r="B23" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="C23" s="8"/>
+      <c r="C23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>106</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="C24" s="8"/>
+        <v>77</v>
+      </c>
+      <c r="C24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B25" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="C25" s="8"/>
+      <c r="C25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="B26" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C26" s="8"/>
+      <c r="C26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>111</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C27" s="8"/>
+        <v>87</v>
+      </c>
+      <c r="C27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="C28" s="8"/>
+        <v>89</v>
+      </c>
+      <c r="C28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="C29" s="8"/>
+        <v>94</v>
+      </c>
+      <c r="C29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="C30" s="8"/>
+        <v>115</v>
+      </c>
+      <c r="C30" s="6"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="C31" s="8"/>
+        <v>99</v>
+      </c>
+      <c r="C31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="C32" s="8"/>
+      <c r="C32" s="6"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="C33" s="8"/>
+      <c r="C33" s="6"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="8"/>
+      <c r="C34" s="6"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="8"/>
+      <c r="C35" s="6"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="8"/>
+      <c r="C36" s="6"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="8"/>
+      <c r="C37" s="6"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="8"/>
+      <c r="C38" s="6"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="8"/>
+      <c r="C39" s="6"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="8"/>
+      <c r="C40" s="6"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="8"/>
+      <c r="C41" s="6"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="8"/>
+      <c r="C42" s="6"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="8"/>
+      <c r="C43" s="6"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="8"/>
+      <c r="C44" s="6"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="8"/>
+      <c r="C45" s="6"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="8"/>
+      <c r="C46" s="6"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C47" s="8"/>
+      <c r="C47" s="6"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C48" s="8"/>
+      <c r="C48" s="6"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C49" s="8"/>
+      <c r="C49" s="6"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C50" s="8"/>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C51" s="8"/>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C52" s="8"/>
-    </row>
+      <c r="C50" s="6"/>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="C3:C52"/>
+  <mergeCells count="1">
+    <mergeCell ref="C1:C50"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1714,7 +1625,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1731,7 +1641,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="9" width="8.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="8.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="70.85"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="4" width="9.14"/>
@@ -1739,398 +1649,398 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C4" s="8"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C5" s="8"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C6" s="8"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C7" s="8"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C8" s="8"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C9" s="8"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C10" s="8"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="C11" s="8"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C12" s="8"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="C13" s="8"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C14" s="8"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C15" s="8"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="C16" s="8"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="B17" s="4" t="s">
+      <c r="B18" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C17" s="8"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B18" s="4" t="s">
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="C18" s="8"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="9" t="s">
+      <c r="B19" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="C19" s="8"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="9" t="s">
+      <c r="B20" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="C20" s="8"/>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="9" t="s">
+      <c r="B21" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="C21" s="8"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="9" t="s">
+      <c r="B22" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="C22" s="6"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="C22" s="8"/>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9" t="s">
+      <c r="B23" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="C23" s="6"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="C23" s="8"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="9" t="s">
+      <c r="B24" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="C24" s="6"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="C24" s="8"/>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="9" t="s">
+      <c r="B25" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="C25" s="8"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="9" t="s">
+      <c r="B26" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="C26" s="8"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="9" t="s">
+      <c r="B27" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="C27" s="6"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="C27" s="8"/>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="9" t="s">
+      <c r="B28" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="C28" s="8"/>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="9" t="s">
+      <c r="B29" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="C29" s="8"/>
+      <c r="C29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="8"/>
+      <c r="C30" s="6"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="8"/>
+      <c r="C31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="8"/>
+      <c r="C32" s="6"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="8"/>
+      <c r="C33" s="6"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="8"/>
+      <c r="C34" s="6"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="8"/>
+      <c r="C35" s="6"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="8"/>
+      <c r="C36" s="6"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="8"/>
+      <c r="C37" s="6"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="8"/>
+      <c r="C38" s="6"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="8"/>
+      <c r="C39" s="6"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="8"/>
+      <c r="C40" s="6"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="8"/>
+      <c r="C41" s="6"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="8"/>
+      <c r="C42" s="6"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="8"/>
+      <c r="C43" s="6"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="8"/>
+      <c r="C44" s="6"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="8"/>
+      <c r="C45" s="6"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="8"/>
+      <c r="C46" s="6"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C47" s="8"/>
+      <c r="C47" s="6"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C48" s="8"/>
+      <c r="C48" s="6"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C49" s="8"/>
+      <c r="C49" s="6"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C50" s="8"/>
+      <c r="C50" s="6"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C51" s="8"/>
+      <c r="C51" s="6"/>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C52" s="8"/>
+      <c r="C52" s="6"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C53" s="8"/>
+      <c r="C53" s="6"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C54" s="8"/>
+      <c r="C54" s="6"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C55" s="8"/>
+      <c r="C55" s="6"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C56" s="8"/>
+      <c r="C56" s="6"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C57" s="8"/>
+      <c r="C57" s="6"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C58" s="8"/>
+      <c r="C58" s="6"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C59" s="8"/>
+      <c r="C59" s="6"/>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C60" s="8"/>
+      <c r="C60" s="6"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C61" s="8"/>
+      <c r="C61" s="6"/>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C62" s="8"/>
+      <c r="C62" s="6"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C63" s="8"/>
+      <c r="C63" s="6"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C64" s="8"/>
+      <c r="C64" s="6"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C65" s="8"/>
+      <c r="C65" s="6"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C66" s="8"/>
+      <c r="C66" s="6"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C67" s="8"/>
+      <c r="C67" s="6"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C68" s="8"/>
+      <c r="C68" s="6"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C69" s="8"/>
+      <c r="C69" s="6"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C70" s="8"/>
+      <c r="C70" s="6"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C71" s="8"/>
+      <c r="C71" s="6"/>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C72" s="8"/>
+      <c r="C72" s="6"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C73" s="8"/>
+      <c r="C73" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>